<commit_message>
modifico funcion de busqueda por dni
</commit_message>
<xml_diff>
--- a/Generador de actas/acta_de_examen.xlsx
+++ b/Generador de actas/acta_de_examen.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,7 +447,7 @@
     <col width="11" customWidth="1" min="4" max="4"/>
     <col width="11" customWidth="1" min="5" max="5"/>
     <col width="7" customWidth="1" min="6" max="6"/>
-    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="25" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -521,6 +521,43 @@
       <c r="G2" s="3" t="inlineStr">
         <is>
           <t>PASANTÍA</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>CAMILA OLMOS</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>45888555</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>MMO</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>REGULAR</t>
+        </is>
+      </c>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>1°2°</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>EDUC. ARTÍSTICA: MÚSICA</t>
         </is>
       </c>
     </row>
@@ -535,14 +572,87 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="7" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="11" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="5" max="5"/>
+    <col width="10" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>ESPACIO CURRICULAR</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>CURSO</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>MODALIDAD</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>CONDICION</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>ALUMNO 1</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>DNI 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>EDUC. ARTÍSTICA: MÚSICA</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>1°2°</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>MMO</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>REGULAR</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="inlineStr">
+        <is>
+          <t>CAMILA OLMOS</t>
+        </is>
+      </c>
+      <c r="F2" s="3" t="inlineStr">
+        <is>
+          <t>45888555</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
se agrega proteccion al archivo de excel
</commit_message>
<xml_diff>
--- a/Generador de actas/acta_de_examen.xlsx
+++ b/Generador de actas/acta_de_examen.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,12 +442,12 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="4" customWidth="1" min="1" max="1"/>
-    <col width="16" customWidth="1" min="2" max="2"/>
-    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="14" customWidth="1" min="2" max="2"/>
+    <col width="5" customWidth="1" min="3" max="3"/>
     <col width="11" customWidth="1" min="4" max="4"/>
     <col width="11" customWidth="1" min="5" max="5"/>
     <col width="7" customWidth="1" min="6" max="6"/>
-    <col width="25" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -495,12 +495,12 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>FRANCO PACHECO</t>
+          <t>CAMILA OLMOS</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>43254999</t>
+          <t>45</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
@@ -521,47 +521,11 @@
       <c r="G2" s="3" t="inlineStr">
         <is>
           <t>PASANTÍA</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>CAMILA OLMOS</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>45888555</t>
-        </is>
-      </c>
-      <c r="D3" s="3" t="inlineStr">
-        <is>
-          <t>MMO</t>
-        </is>
-      </c>
-      <c r="E3" s="3" t="inlineStr">
-        <is>
-          <t>REGULAR</t>
-        </is>
-      </c>
-      <c r="F3" s="3" t="inlineStr">
-        <is>
-          <t>1°2°</t>
-        </is>
-      </c>
-      <c r="G3" s="3" t="inlineStr">
-        <is>
-          <t>EDUC. ARTÍSTICA: MÚSICA</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="C6D3"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -572,87 +536,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="25" customWidth="1" min="1" max="1"/>
-    <col width="7" customWidth="1" min="2" max="2"/>
-    <col width="11" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
-    <col width="14" customWidth="1" min="5" max="5"/>
-    <col width="10" customWidth="1" min="6" max="6"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>ESPACIO CURRICULAR</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>CURSO</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>MODALIDAD</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>CONDICION</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>ALUMNO 1</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>DNI 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t>EDUC. ARTÍSTICA: MÚSICA</t>
-        </is>
-      </c>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
-          <t>1°2°</t>
-        </is>
-      </c>
-      <c r="C2" s="3" t="inlineStr">
-        <is>
-          <t>MMO</t>
-        </is>
-      </c>
-      <c r="D2" s="3" t="inlineStr">
-        <is>
-          <t>REGULAR</t>
-        </is>
-      </c>
-      <c r="E2" s="3" t="inlineStr">
-        <is>
-          <t>CAMILA OLMOS</t>
-        </is>
-      </c>
-      <c r="F2" s="3" t="inlineStr">
-        <is>
-          <t>45888555</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -675,8 +566,8 @@
     <col width="7" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
     <col width="11" customWidth="1" min="4" max="4"/>
-    <col width="16" customWidth="1" min="5" max="5"/>
-    <col width="10" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="5" max="5"/>
+    <col width="7" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -734,12 +625,12 @@
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>FRANCO PACHECO</t>
+          <t>CAMILA OLMOS</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>43254999</t>
+          <t>45</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
soluciono el problema de que para materis que son del ciclo basico se generaban actas para las dos especialidades cuando el alumno pertenencia a solamente una
</commit_message>
<xml_diff>
--- a/Generador de actas/acta_de_examen.xlsx
+++ b/Generador de actas/acta_de_examen.xlsx
@@ -57,16 +57,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -440,87 +434,74 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="4" customWidth="1" min="1" max="1"/>
-    <col width="14" customWidth="1" min="2" max="2"/>
-    <col width="5" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
-    <col width="11" customWidth="1" min="5" max="5"/>
-    <col width="7" customWidth="1" min="6" max="6"/>
-    <col width="20" customWidth="1" min="7" max="7"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>N°</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>ALUMNO</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>DNI</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>MODALIDAD</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>CONDICION</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>CURSO</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>ESPACIO CURRICULAR</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
-          <t>CAMILA OLMOS</t>
-        </is>
-      </c>
-      <c r="C2" s="3" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="D2" s="3" t="inlineStr">
-        <is>
-          <t>TEM</t>
-        </is>
-      </c>
-      <c r="E2" s="3" t="inlineStr">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>55</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>MMO</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>REGULAR</t>
         </is>
       </c>
-      <c r="F2" s="3" t="inlineStr">
-        <is>
-          <t>7°2°</t>
-        </is>
-      </c>
-      <c r="G2" s="3" t="inlineStr">
-        <is>
-          <t>PASANTÍA</t>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1°1°</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>LENGUA Y LITERATURA I (MMO)</t>
         </is>
       </c>
     </row>
@@ -531,6 +512,87 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ESPACIO CURRICULAR</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>CURSO</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>MODALIDAD</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>CONDICION</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ALUMNO 1</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>DNI 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>LENGUA Y LITERATURA I (MMO)</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1°1°</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>MMO</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>REGULAR</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -546,95 +608,4 @@
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="7" customWidth="1" min="2" max="2"/>
-    <col width="11" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
-    <col width="14" customWidth="1" min="5" max="5"/>
-    <col width="7" customWidth="1" min="6" max="6"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>ESPACIO CURRICULAR</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>CURSO</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>MODALIDAD</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>CONDICION</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>ALUMNO 1</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>DNI 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t>PASANTÍA</t>
-        </is>
-      </c>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
-          <t>7°2°</t>
-        </is>
-      </c>
-      <c r="C2" s="3" t="inlineStr">
-        <is>
-          <t>TEM</t>
-        </is>
-      </c>
-      <c r="D2" s="3" t="inlineStr">
-        <is>
-          <t>REGULAR</t>
-        </is>
-      </c>
-      <c r="E2" s="3" t="inlineStr">
-        <is>
-          <t>CAMILA OLMOS</t>
-        </is>
-      </c>
-      <c r="F2" s="3" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
agrego funcionalidad para agregar materias
</commit_message>
<xml_diff>
--- a/Generador de actas/acta_de_examen.xlsx
+++ b/Generador de actas/acta_de_examen.xlsx
@@ -57,10 +57,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -434,78 +440,92 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="4" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="11" customWidth="1" min="4" max="4"/>
+    <col width="11" customWidth="1" min="5" max="5"/>
+    <col width="7" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>N°</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>ALUMNO</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>DNI</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>MODALIDAD</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>CONDICION</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>CURSO</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>ESPACIO CURRICULAR</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>AMIRA YARBOUH</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>17599256</v>
-      </c>
-      <c r="D2" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>17599256</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
         <is>
           <t>MMO</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="3" t="inlineStr">
         <is>
           <t>REGULAR</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="3" t="inlineStr">
         <is>
           <t>1°1°</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" s="3" t="inlineStr">
         <is>
           <t>GEOGRAFÍA I</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="C6D3"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -523,72 +543,85 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="4" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="11" customWidth="1" min="4" max="4"/>
+    <col width="11" customWidth="1" min="5" max="5"/>
+    <col width="7" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>N°</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>ALUMNO</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>DNI</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>MODALIDAD</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>CONDICION</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>CURSO</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>ESPACIO CURRICULAR</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>AMIRA YARBOUH</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>17599256</v>
-      </c>
-      <c r="D2" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>17599256</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
         <is>
           <t>MMO</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="3" t="inlineStr">
         <is>
           <t>REGULAR</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="3" t="inlineStr">
         <is>
           <t>1°1°</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" s="3" t="inlineStr">
         <is>
           <t>GEOGRAFÍA I</t>
         </is>
@@ -612,72 +645,85 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="4" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="11" customWidth="1" min="4" max="4"/>
+    <col width="11" customWidth="1" min="5" max="5"/>
+    <col width="7" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>N°</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>ALUMNO</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>DNI</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>MODALIDAD</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>CONDICION</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>CURSO</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>ESPACIO CURRICULAR</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>AMIRA YARBOUH</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>17599256</v>
-      </c>
-      <c r="D2" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>17599256</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
         <is>
           <t>MMO</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="3" t="inlineStr">
         <is>
           <t>REGULAR</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="3" t="inlineStr">
         <is>
           <t>1°1°</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" s="3" t="inlineStr">
         <is>
           <t>GEOGRAFÍA I</t>
         </is>

</xml_diff>